<commit_message>
Changes that are simpler and support new requirements
</commit_message>
<xml_diff>
--- a/data/BillingRates.xlsx
+++ b/data/BillingRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dkinney/dev/midi/embassyInvoices/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB05333-8C68-274C-A028-286EB8978F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8948C774-9050-D749-A220-5442A098037E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="500" windowWidth="37200" windowHeight="24420" xr2:uid="{951AFB9B-BA60-164C-8B3E-C7B59A408681}"/>
+    <workbookView xWindow="3060" yWindow="500" windowWidth="26000" windowHeight="17060" xr2:uid="{951AFB9B-BA60-164C-8B3E-C7B59A408681}"/>
   </bookViews>
   <sheets>
     <sheet name="Labor Rates" sheetId="1" r:id="rId1"/>
@@ -1535,8 +1535,8 @@
   <dimension ref="A1:G170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C103" sqref="A103:XFD103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>